<commit_message>
Updated Learn tab to offer more information and updated to do list
</commit_message>
<xml_diff>
--- a/Database - Learn.xlsx
+++ b/Database - Learn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GraceMaloney/Downloads/HCI 584X/Project/Code/National-Park-Journal-and-Learn_HCI584/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9DE158-C5AA-354F-8AA6-5AAF4200A0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91609DC0-7A46-DF4B-AC61-EF423E38C61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{21CDAEF0-8EF3-284B-980A-1BFB33ABAC9E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="532">
   <si>
     <t>Name</t>
   </si>
@@ -1478,6 +1478,299 @@
   <si>
     <t>Hiking, bear viewing, camping, backpacking, kayaking, fishing, rafting</t>
   </si>
+  <si>
+    <t>National Park Photos/Bryce Canyon National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/brca/index.htm</t>
+  </si>
+  <si>
+    <t>Bryce Canyon is a geological amphitheater on southern Utah's Paunsaugunt Plateau with hundreds of tall, multicolored sandstone hoodoos formed by erosion. The region was originally settled by Native Americans and later by Mormon pioneers.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Canyonlands National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/cany/index.htm</t>
+  </si>
+  <si>
+    <t>This landscape was eroded into a maze of canyons, buttes, and mesas by the combined efforts of the Colorado River, Green River, and their tributaries, which divide the park into three districts. The park contains thousands of rock pinnacles and arches, as well as artifacts from Ancient Pueblo peoples.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Capitol Reef National Park.jpeg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/care/index.htm</t>
+  </si>
+  <si>
+    <t>The park's Waterpocket Fold is a 100-mile (160 km) monocline that exhibits the earth's diverse geologic layers. Other natural features include monoliths, eroded buttes, and sandstone domes, including one shaped like the United States Capitol.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Carlsbad Caverns National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/cave/index.htm</t>
+  </si>
+  <si>
+    <t>Carlsbad Caverns has 117 caves, the longest of which is over 120 miles (190 km) long. The Big Room is almost 4,000 feet (1,200 m) long, and the caves are home to over 400,000 Mexican free-tailed bats and sixteen other species. Above ground are the Chihuahuan Desert and Rattlesnake Springs.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Channel Islands National Park.jpeg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/chis/index.htm</t>
+  </si>
+  <si>
+    <t>Five of the eight Channel Islands are protected, with half of the park's area underwater. The islands have a unique Mediterranean ecosystem originally settled by the Chumash people. They are home to over 2,000 species of land plants and animals, 145 endemic to them, including the island fox. Ferry services offer transportation to the islands from the mainland.</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>National Park Photos/Congaree National Park.jpeg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/cong/index.htm</t>
+  </si>
+  <si>
+    <t>On the Congaree River, this park is the largest portion of old-growth floodplain forest left in North America. Some of the trees are the tallest in the eastern United States. An elevated walkway called the Boardwalk Loop guides visitors through the swamp.</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>National Park Photos/Crater Lake National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/crla/index.htm</t>
+  </si>
+  <si>
+    <t>Crater Lake lies in the caldera of an ancient volcano called Mount Mazama that collapsed 7,700 years ago. The lake is the deepest in the United States and is noted for its vivid blue color and water clarity. Wizard Island and the Phantom Ship are more recent volcanic formations within the caldera. As the lake has no inlets or outlets, it is replenished only by precipitation.</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>National Park Photos/Cuyahoga Valley National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/cuva/index.htm</t>
+  </si>
+  <si>
+    <t>This park along the Cuyahoga River has waterfalls, hills, trails, and exhibits on early rural living. The Ohio and Erie Canal Towpath Trail follows the Ohio and Erie Canal, where mules towed canal boats. The park has numerous historic homes, bridges, and structures, and also offers a scenic train ride.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Death Valley National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/deva/index.htm</t>
+  </si>
+  <si>
+    <t>Death Valley is the hottest, lowest, and driest place in the United States, with daytime temperatures that have exceeded 130 °F (54 °C). The park protects Badwater Basin and its vast salt flats at the lowest elevation in North America, −282 ft (−86 m). This geologic graben also protects numerous canyons, badlands, sand dunes, mountain ranges, historic mines, springs, and more than 1,000 species of plants that grow.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Dry Tortugas National Park.jpeg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/drto/index.htm</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>The islands of the Dry Tortugas, at the westernmost end of the Florida Keys, are the site of Fort Jefferson, a Civil War-era fort that is the largest masonry structure in the Western Hemisphere. The park is home to undisturbed coral reefs and shipwrecks, and is only accessible by plane or boat.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Everglades National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/ever/index.htm</t>
+  </si>
+  <si>
+    <t>The Everglades are the largest tropical wilderness in the United States. This mangrove and tropical rainforest ecosystem and marine estuary is home to 36 protected species, including the Florida panther, American crocodile, and West Indian manatee. Some areas have been drained and developed; restoration projects aim to restore the ecology.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Gates of the Arctic National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/gaar/index.htm</t>
+  </si>
+  <si>
+    <t>The country's northernmost park protects an expanse of pure wilderness in Alaska's Brooks Range and has no park facilities. The land is home to Alaska Natives who have relied on the land and caribou for 11,000 years.</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>National Park Photos/Gateway Arch National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/jeff/index.htm</t>
+  </si>
+  <si>
+    <r>
+      <t>The Gateway Arch is a 630-foot (192 m) (both high and wide) catenary arch built in the 1960s to commemorate the Lewis and Clark Expedition, initiated by Thomas Jefferson, and the subsequent westward expansion of the country. The nearby Old Courthouse, across a greenway to the west of the arch, was the original site of the landmark </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dred Scott</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> case about slavery. An underground museum describes the arch's construction and the country's westward expansion.</t>
+    </r>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>National Park Photos/Great Basin National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/grba/index.htm</t>
+  </si>
+  <si>
+    <t>Based around Nevada's second tallest mountain, Wheeler Peak, Great Basin National Park protects 5,000-year-old bristlecone pines, a rock glacier, and the limestone Lehman Caves. Due to its remote location, the park is home to some of the country's darkest night skies. Wildlife includes the Townsend's big-eared bat, pronghorn, and Bonneville cutthroat trout.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Great Sand Dunes National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/grsa/index.htm</t>
+  </si>
+  <si>
+    <t>The tallest sand dunes in North America, up to 750 feet (230 m) tall, were formed by deposits of the ancient Rio Grande in the San Luis Valley. Abutting a variety of grasslands, shrublands, and wetlands, the park also features alpine lakes, six 13,000-foot mountains, and old-growth forests.</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>National Park Photos/Great Smoky Mountains National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/grsm/index.htm</t>
+  </si>
+  <si>
+    <t>The Great Smoky Mountains, part of the Appalachian Mountains, span a wide range of elevations, making them home to over 400 vertebrate species, 100 tree species, and 5,000 plant species. Hiking is the park's main attraction, with over 800 miles (1,300 km) of trails, including 70 miles (110 km) of the Appalachian Trail. Other activities include fishing, horseback riding, and touring nearly 80 historic structures.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Guadalupe Mountains National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/gumo/index.htm</t>
+  </si>
+  <si>
+    <t>This park contains Guadalupe Peak, the highest point in Texas, as well as the scenic McKittrick Canyon filled with bigtooth maples, a corner of the arid Chihuahuan Desert, and a fossilized coral reef from the Permian era.</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>National Park Photos/Haleakala National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/hale/index.htm</t>
+  </si>
+  <si>
+    <t>The Haleakalā volcano on Maui features a very large crater with numerous cinder cones, a grove of non-native trees, the Kipahulu section's scenic pools of freshwater fish, and the endemic Hawaiian goose. The park protects the greatest number of endangered species within a U.S. national park.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Hawai’i Volcanoes National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/havo/index.htm</t>
+  </si>
+  <si>
+    <t>This park on the Big Island protects the Kīlauea and Mauna Loa volcanoes, two of the world's most active geological features. Diverse ecosystems range from tropical forests at sea level to barren lava beds at more than 13,000 feet (4,000 m).</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>National Park Photos/Hot Springs National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/hosp/index.htm</t>
+  </si>
+  <si>
+    <t>Hot Springs was originally established by Congress as a federal reserve on April 20, 1832, making it the oldest area managed by the National Park Service. Natural thermal springs flow out of the Ouachita Mountains, providing opportunities for relaxation in a historic setting. Bathhouse Row preserves examples of 19th-century architecture. Hot Springs is the first national park within a city and was the smallest national park until 2018.</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>National Park Photos/Indiana Dunes National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/indu/index.htm</t>
+  </si>
+  <si>
+    <t>Previously designated a national lakeshore, parts of this 20-mile (32 km) stretch of the southern shore of Lake Michigan have sandy beaches and tall dunes. The park includes grassy prairies, peat bogs, and marsh wetlands home to over 2,000 species.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Joshua Tree National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/jotr/index.htm</t>
+  </si>
+  <si>
+    <t>Covering large areas of the Colorado and Mojave Deserts and the Little San Bernardino Mountains, this desert landscape is populated by vast stands of Joshua trees. Large changes in elevation reveal various contrasting environments including bleached sand dunes, dry lakes, rugged mountains, and maze-like clusters of monzogranite monoliths.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Katmai National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/katm/index.htm</t>
+  </si>
+  <si>
+    <t>This park on the Alaska Peninsula protects the Valley of Ten Thousand Smokes, an ash flow formed by the 1912 eruption of Novarupta, and the stratovolcano Mount Katmai. Over 2,000 grizzly bears come here each year to catch spawning salmon. Other wildlife includes caribou, wolves, moose, and wolverines.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Kenai Fjords National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/kefj/index.htm</t>
+  </si>
+  <si>
+    <t>Near Seward on the Kenai Peninsula, this park protects the Harding Icefield and at least 38 glaciers and fjords stemming from it. The only area accessible to the public by road is the rapidly shrinking Exit Glacier. Boat and kayak tours offer views of tidewater glaciers, whales, sea lions, and marine birds.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Kings Canyon National Park.jpg</t>
+  </si>
+  <si>
+    <t>Home to several giant sequoia groves and the General Grant Tree, the world's second largest measured tree, this park also features part of the Kings River, sculptor of the dramatic granite canyon that is its namesake, and the San Joaquin River, as well as Boyden Cave. Although Kings Canyon National Park was designated as such in 1940, it subsumed General Grant National Park, which had been established on October 1, 1890, as the United States' fourth national park.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Kobuk Valley National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/kova/index.htm</t>
+  </si>
+  <si>
+    <t>Kobuk Valley protects 61 miles (98 km) of the Kobuk River and three regions of sand dunes. Created by glaciers, the Great Kobuk, Little Kobuk, and Hunt River Sand Dunes can reach 100 feet (30 m) high and 100 °F (38 °C), and they are the largest dunes in the Arctic. Twice a year, half a million caribou migrate through the dunes and across river bluffs that expose well-preserved ice age fossils.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Lake Clark National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/lacl/index.htm</t>
+  </si>
+  <si>
+    <t>The region around Lake Clark features four active volcanoes, including Mount Redoubt, as well as an abundance of rivers, glaciers, and waterfalls. Temperate rainforests, a tundra plateau, and three mountain ranges complete the landscape.</t>
+  </si>
 </sst>
 </file>
 
@@ -1486,7 +1779,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1539,6 +1832,14 @@
     </font>
     <font>
       <vertAlign val="superscript"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1898,19 +2199,19 @@
   <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" style="2" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="67.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="25.1640625" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="119.1640625" style="2" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="44.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="25.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="119.1640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="33.5" style="2" customWidth="1"/>
     <col min="10" max="10" width="56.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.1640625" style="2" customWidth="1"/>
@@ -2232,26 +2533,26 @@
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>15</v>
+        <v>442</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="E8" s="6">
+        <v>35</v>
+      </c>
+      <c r="F8" s="6">
+        <v>20</v>
+      </c>
+      <c r="G8" s="6">
+        <v>30</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>444</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>254</v>
@@ -2276,26 +2577,26 @@
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>16</v>
+        <v>445</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="E9" s="6">
+        <v>30</v>
+      </c>
+      <c r="F9" s="6">
+        <v>15</v>
+      </c>
+      <c r="G9" s="6">
+        <v>25</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>447</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>261</v>
@@ -2320,26 +2621,26 @@
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>17</v>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>17</v>
+        <v>448</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="E10" s="6">
+        <v>20</v>
+      </c>
+      <c r="F10" s="6">
+        <v>10</v>
+      </c>
+      <c r="G10" s="6">
+        <v>15</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>450</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>262</v>
@@ -2365,25 +2666,25 @@
         <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>18</v>
+        <v>451</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="E11" s="6">
+        <v>30</v>
+      </c>
+      <c r="F11" s="6">
+        <v>15</v>
+      </c>
+      <c r="G11" s="6">
+        <v>25</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>453</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>272</v>
@@ -2408,26 +2709,26 @@
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>20</v>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>20</v>
+        <v>454</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>456</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>274</v>
@@ -2453,25 +2754,25 @@
         <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>22</v>
+        <v>457</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>22</v>
+        <v>458</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>460</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>284</v>
@@ -2497,25 +2798,25 @@
         <v>23</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>23</v>
+        <v>461</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>23</v>
+        <v>462</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="E14" s="6">
+        <v>30</v>
+      </c>
+      <c r="F14" s="6">
+        <v>15</v>
+      </c>
+      <c r="G14" s="6">
+        <v>25</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>464</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>290</v>
@@ -2541,25 +2842,25 @@
         <v>24</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>465</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>24</v>
+        <v>466</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>468</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>297</v>
@@ -2584,26 +2885,26 @@
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="E16" s="6">
+        <v>30</v>
+      </c>
+      <c r="F16" s="6">
+        <v>15</v>
+      </c>
+      <c r="G16" s="6">
         <v>25</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>25</v>
+      <c r="H16" s="2" t="s">
+        <v>471</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>302</v>
@@ -2673,25 +2974,25 @@
         <v>28</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>28</v>
+        <v>472</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="F18" s="6">
+        <v>15</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>475</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>309</v>
@@ -2717,25 +3018,25 @@
         <v>29</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>29</v>
+        <v>476</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="E19" s="6">
+        <v>30</v>
+      </c>
+      <c r="F19" s="6">
+        <v>15</v>
+      </c>
+      <c r="G19" s="6">
+        <v>25</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>478</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>314</v>
@@ -2761,25 +3062,25 @@
         <v>30</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>30</v>
+        <v>479</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>481</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>320</v>
@@ -2805,25 +3106,25 @@
         <v>31</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>31</v>
+        <v>482</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>31</v>
+        <v>483</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>485</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>325</v>
@@ -3024,26 +3325,26 @@
       <c r="A26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>39</v>
+      <c r="B26" s="2" t="s">
+        <v>486</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>39</v>
+        <v>487</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0</v>
+      </c>
+      <c r="G26" s="6">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>489</v>
       </c>
       <c r="I26" s="3" t="s">
         <v>357</v>
@@ -3069,25 +3370,25 @@
         <v>40</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>40</v>
+        <v>490</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="E27" s="6">
+        <v>25</v>
+      </c>
+      <c r="F27" s="6">
+        <v>15</v>
+      </c>
+      <c r="G27" s="6">
+        <v>20</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>492</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>363</v>
@@ -3113,25 +3414,25 @@
         <v>41</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>41</v>
+        <v>493</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>41</v>
+        <v>494</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0</v>
+      </c>
+      <c r="G28" s="6">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>496</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>369</v>
@@ -3157,25 +3458,25 @@
         <v>42</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>42</v>
+        <v>497</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="E29" s="6">
+        <v>20</v>
+      </c>
+      <c r="F29" s="6">
+        <v>10</v>
+      </c>
+      <c r="G29" s="6">
+        <v>15</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>499</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>375</v>
@@ -3201,25 +3502,25 @@
         <v>43</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>43</v>
+        <v>500</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>43</v>
+        <v>501</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E30" s="6">
+        <v>30</v>
+      </c>
+      <c r="F30" s="6">
+        <v>15</v>
+      </c>
+      <c r="G30" s="6">
+        <v>25</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>503</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>377</v>
@@ -3245,25 +3546,25 @@
         <v>44</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>44</v>
+        <v>500</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>44</v>
+        <v>504</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="E31" s="6">
+        <v>30</v>
+      </c>
+      <c r="F31" s="6">
+        <v>15</v>
+      </c>
+      <c r="G31" s="6">
+        <v>25</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>506</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>387</v>
@@ -3289,25 +3590,25 @@
         <v>45</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>45</v>
+        <v>507</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>45</v>
+        <v>508</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0</v>
+      </c>
+      <c r="F32" s="6">
+        <v>0</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>510</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>388</v>
@@ -3333,25 +3634,25 @@
         <v>46</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>46</v>
+        <v>511</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>46</v>
+        <v>512</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E33" s="6">
+        <v>25</v>
+      </c>
+      <c r="F33" s="6">
+        <v>15</v>
+      </c>
+      <c r="G33" s="6">
+        <v>20</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>514</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>398</v>
@@ -3420,26 +3721,26 @@
       <c r="A35" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>48</v>
+      <c r="B35" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>48</v>
+        <v>515</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="E35" s="6">
+        <v>30</v>
+      </c>
+      <c r="F35" s="6">
+        <v>15</v>
+      </c>
+      <c r="G35" s="6">
+        <v>25</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>517</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>411</v>
@@ -3465,25 +3766,25 @@
         <v>49</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>49</v>
+        <v>518</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="E36" s="6">
+        <v>0</v>
+      </c>
+      <c r="F36" s="6">
+        <v>0</v>
+      </c>
+      <c r="G36" s="6">
+        <v>0</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>520</v>
       </c>
       <c r="I36" s="3" t="s">
         <v>416</v>
@@ -3509,25 +3810,25 @@
         <v>50</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>50</v>
+        <v>521</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0</v>
+      </c>
+      <c r="F37" s="6">
+        <v>0</v>
+      </c>
+      <c r="G37" s="6">
+        <v>0</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>523</v>
       </c>
       <c r="I37" s="3" t="s">
         <v>422</v>
@@ -3552,26 +3853,26 @@
       <c r="A38" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>51</v>
+      <c r="B38" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>51</v>
+        <v>524</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E38" s="6">
+        <v>35</v>
+      </c>
+      <c r="F38" s="6">
+        <v>20</v>
+      </c>
+      <c r="G38" s="6">
+        <v>30</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>525</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>429</v>
@@ -3597,25 +3898,25 @@
         <v>52</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>52</v>
+        <v>526</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="E39" s="6">
+        <v>0</v>
+      </c>
+      <c r="F39" s="6">
+        <v>0</v>
+      </c>
+      <c r="G39" s="6">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>528</v>
       </c>
       <c r="I39" s="3" t="s">
         <v>434</v>
@@ -3641,25 +3942,25 @@
         <v>53</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>53</v>
+        <v>529</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="E40" s="6">
+        <v>0</v>
+      </c>
+      <c r="F40" s="6">
+        <v>0</v>
+      </c>
+      <c r="G40" s="6">
+        <v>0</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>531</v>
       </c>
       <c r="I40" s="3" t="s">
         <v>440</v>

</xml_diff>

<commit_message>
Updated database to include more information
</commit_message>
<xml_diff>
--- a/Database - Learn.xlsx
+++ b/Database - Learn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GraceMaloney/Downloads/HCI 584X/Project/Code/National-Park-Journal-and-Learn_HCI584/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91609DC0-7A46-DF4B-AC61-EF423E38C61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93017782-5B6C-B747-93AA-5806F3D1C24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{21CDAEF0-8EF3-284B-980A-1BFB33ABAC9E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="670">
   <si>
     <t>Name</t>
   </si>
@@ -780,9 +780,6 @@
     <t>https://www.nps.gov/dena/planyourvisit/things2do.htm</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>https://www.nps.gov/dena/learn/nature/wildlife.htm</t>
   </si>
   <si>
@@ -1770,6 +1767,423 @@
   </si>
   <si>
     <t>The region around Lake Clark features four active volcanoes, including Mount Redoubt, as well as an abundance of rivers, glaciers, and waterfalls. Temperate rainforests, a tundra plateau, and three mountain ranges complete the landscape.</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/lavo/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/lavo/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/lavo/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Black bears, sierra neveda red foxes, moutain lions, pikas, otters</t>
+  </si>
+  <si>
+    <t>Hiking, backpacking, biking, kayaking, fishing, swimming</t>
+  </si>
+  <si>
+    <t>Lassen Volcanic National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/maca/planyourvisit/operatinghoursandseasons.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/maca/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/maca/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Bats, skinks, bullfrogs, turtles</t>
+  </si>
+  <si>
+    <t>Cave touring, biking, hiking, kayaking, canoeing, fishing</t>
+  </si>
+  <si>
+    <t>Mammoth Cave National Park is open year-round.</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/meve/planyourvisit/basicinfo.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/meve/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/meve/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Mexican spotted owls, elk, black bears, bats, rattlesnakes, weasels</t>
+  </si>
+  <si>
+    <t>Hiking, camping, cliff dwelling tours</t>
+  </si>
+  <si>
+    <t>Mesa Verde National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Mount Rainier National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/mora/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/mora/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/mora/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Black bears, cascade red foxes, moutain lions, elk, mountain goats, moose</t>
+  </si>
+  <si>
+    <t>Hiking, camping, rock climbing, biking, fishing, mountaineering</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/npsa/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/npsa/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/npsa/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Humpback whales, sperm whales, orcas, dolphins, sea turtles, geckos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The National Park of American Samoa is open year-round, but some areas of the park may be temporarily closed due to trail maintenance or safety measures.</t>
+  </si>
+  <si>
+    <t>Fishing, snorkeling, hiking, diving, beachwalking</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/neri/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/neri/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/neri/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Whitewater rafting, hiking, camping, biking, rock climbing, fishing</t>
+  </si>
+  <si>
+    <t>Black bears, red foxes, beavers, minks, river otters</t>
+  </si>
+  <si>
+    <t>New River Gorge National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/noca/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/noca/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/noca/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Mountain goats, bighorn sheep, elk, moose, gray wolves, red foxes, river otters</t>
+  </si>
+  <si>
+    <t>Hiking, backpacking, camping, canoeing, kayaking, biking, mountaineering</t>
+  </si>
+  <si>
+    <t>North Cascades National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/olym/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/olym/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/olym/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Whales, dolphins, sea lions, seals, sea otters, elk, black bears</t>
+  </si>
+  <si>
+    <t>Kayaking, fishing, camping, hiking, backpacking, climbing, skiing</t>
+  </si>
+  <si>
+    <t>Olympic National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/pefo/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/pefo/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/pefo/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Kit foxes, coyote, pronghorn, badgers, bobcats</t>
+  </si>
+  <si>
+    <t>Petrified Forest National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Hiking, backpacking, camping, biking, geocaching</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/pinn/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/pinn/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/pinn/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Canyon bats, mountain lions, condors, foxes, badgers, bobcats</t>
+  </si>
+  <si>
+    <t>Hiking, camping, rock climbing, bird watching</t>
+  </si>
+  <si>
+    <t>Pinnacles National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/redw/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/redw/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/redw/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Elk, mountain beavers, mountain lions, black bears, gray whales, sea lions, elephant seals, orcas, humpback whales, condors</t>
+  </si>
+  <si>
+    <t>Biking, hiking, camping, kayaking</t>
+  </si>
+  <si>
+    <t>Redwood National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/romo/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/romo/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/romo/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Hiking, camping, backpacking, scenic driving, fishing</t>
+  </si>
+  <si>
+    <t>Bighorn sheep, moose, black bears, mountain lions, elk, beavers</t>
+  </si>
+  <si>
+    <t>Rocky Mountain National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/sagu/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/sagu/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/sagu/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Bobcats, packrats, gray foxes, mountain lions, javelinas</t>
+  </si>
+  <si>
+    <t>Camping, hiking, biking</t>
+  </si>
+  <si>
+    <t>Saguaro National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Sequoia National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/shen/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/shen/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Black bears, bobcats, bats, deer, shrews</t>
+  </si>
+  <si>
+    <t>Shenandoah National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/shen/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>Hiking, backcountry camping, scenic driving, fishing, biking</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/thro/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/thro/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/thro/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Bison, wild horses, elk, deer, pronghorn, prairie dogs</t>
+  </si>
+  <si>
+    <t>Theodore Roosevelt National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Scenic driving, hiking, camping</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/viis/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/viis/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/viis/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Sea turtles, nurse sharks, whale sharks, stingrays</t>
+  </si>
+  <si>
+    <t>Virgin Islands National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Snorkeling, swimming, fishing, hiking, boating</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/voya/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/voya/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/voya/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Moose, beavers, wolves, otters, sturgeon, bears</t>
+  </si>
+  <si>
+    <t>Voyageurs National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Canoeing, hiking, boating, snowshoeing, cross-country skiing, fishing, camping</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/whsa/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/whsa/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/whsa/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Badgers, apache pocket mice, bobcats, kit foxes, bats, gophers</t>
+  </si>
+  <si>
+    <t>White Sands National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Sledding, hiking, biking, backcountry camping, dune driving</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/wica/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/wica/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/wica/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Bison, prairie dogs, ferrets, elk, pronghorn</t>
+  </si>
+  <si>
+    <t>Hiking, cave exploring, cave tours</t>
+  </si>
+  <si>
+    <t>Wind Cave National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/wrst/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/wrst/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Polar bears, moose, mountain goats, caribou, black bears, grizzly/brown bears, sea lions</t>
+  </si>
+  <si>
+    <t>Backpacking, mountaineering, boating, fishing, hiking, cross-country skiing</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/wrst/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>Wrangell St. Elias National Park is open year-round, with visitation most popular from May through September</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/yell/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/yell/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/yell/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Black bears, bobcats, lynx, badgers, gray wolves, grizzly bears, foxes, river otters</t>
+  </si>
+  <si>
+    <t>Hiking, camping, biking, scenic driving, cross-country skiing, snowshoeing</t>
+  </si>
+  <si>
+    <t>Yellowstone National Park is open year-round, but facilities are limited or closed during winter months</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/yose/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/yose/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/yose/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Black bears, bighorn sheep, red foxes, pacific fishers, mountain lions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yosemite National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Camping, hiking, backpacking, biking, fishing, rock climbing, swimming, kayaking</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/zion/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/zion/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/zion/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Foxes, black bears, ringtail, badgers, mountain lions, elk, bighorn sheep</t>
+  </si>
+  <si>
+    <t>Backpacking, hiking, river hiking, camping, canyoneering, rock climbing, kayaking, biking</t>
+  </si>
+  <si>
+    <t>Zion National Park is open year-round</t>
   </si>
 </sst>
 </file>
@@ -2198,8 +2612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC95574-44B1-8347-90F2-3758EB862849}">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2291,22 +2705,22 @@
         <v>127</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2335,22 +2749,22 @@
         <v>129</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2379,22 +2793,22 @@
         <v>160</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2423,22 +2837,22 @@
         <v>130</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2467,22 +2881,22 @@
         <v>131</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2511,22 +2925,22 @@
         <v>132</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J7" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>246</v>
-      </c>
       <c r="N7" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2537,10 +2951,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="E8" s="6">
         <v>35</v>
@@ -2552,25 +2966,25 @@
         <v>30</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I8" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>255</v>
-      </c>
       <c r="N8" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2581,10 +2995,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>445</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>446</v>
       </c>
       <c r="E9" s="6">
         <v>30</v>
@@ -2596,25 +3010,25 @@
         <v>25</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J9" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="N9" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2625,10 +3039,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>448</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>449</v>
       </c>
       <c r="E10" s="6">
         <v>20</v>
@@ -2640,25 +3054,25 @@
         <v>15</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I10" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="N10" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2669,10 +3083,10 @@
         <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>451</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>452</v>
       </c>
       <c r="E11" s="6">
         <v>30</v>
@@ -2684,25 +3098,25 @@
         <v>25</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I11" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="M11" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="N11" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2713,40 +3127,40 @@
         <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="E12" s="6">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>456</v>
-      </c>
       <c r="I12" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2754,43 +3168,43 @@
         <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="6">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="E13" s="6">
-        <v>0</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0</v>
-      </c>
-      <c r="G13" s="6">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>460</v>
-      </c>
       <c r="I13" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="M13" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>285</v>
-      </c>
       <c r="N13" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2798,13 +3212,13 @@
         <v>23</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>462</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>463</v>
       </c>
       <c r="E14" s="6">
         <v>30</v>
@@ -2816,25 +3230,25 @@
         <v>25</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I14" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="M14" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>291</v>
-      </c>
       <c r="N14" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2842,43 +3256,43 @@
         <v>24</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="E15" s="6">
-        <v>0</v>
-      </c>
-      <c r="F15" s="6">
-        <v>0</v>
-      </c>
-      <c r="G15" s="6">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>468</v>
-      </c>
       <c r="I15" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J15" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2889,10 +3303,10 @@
         <v>21</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>470</v>
       </c>
       <c r="E16" s="6">
         <v>30</v>
@@ -2904,25 +3318,25 @@
         <v>25</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I16" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="M16" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>303</v>
-      </c>
       <c r="N16" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2951,19 +3365,19 @@
         <v>133</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>203</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>208</v>
@@ -2977,40 +3391,40 @@
         <v>12</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="6" t="s">
         <v>473</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>474</v>
       </c>
       <c r="F18" s="6">
         <v>15</v>
       </c>
       <c r="G18" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>475</v>
-      </c>
       <c r="I18" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J18" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="N18" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3021,10 +3435,10 @@
         <v>12</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>476</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>477</v>
       </c>
       <c r="E19" s="6">
         <v>30</v>
@@ -3036,25 +3450,25 @@
         <v>25</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I19" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="M19" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="J19" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="M19" s="7" t="s">
-        <v>315</v>
-      </c>
       <c r="N19" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3065,40 +3479,40 @@
         <v>27</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="6">
+        <v>0</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="E20" s="6">
-        <v>0</v>
-      </c>
-      <c r="F20" s="6">
-        <v>0</v>
-      </c>
-      <c r="G20" s="6">
-        <v>0</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>481</v>
-      </c>
       <c r="I20" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="M20" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="N20" s="2" t="s">
         <v>316</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3106,43 +3520,43 @@
         <v>31</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="6">
+        <v>0</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="E21" s="6">
-        <v>0</v>
-      </c>
-      <c r="F21" s="6">
-        <v>0</v>
-      </c>
-      <c r="G21" s="6">
-        <v>0</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>485</v>
-      </c>
       <c r="I21" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="M21" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="L21" s="2" t="s">
+      <c r="N21" s="2" t="s">
         <v>323</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3171,22 +3585,22 @@
         <v>126</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J22" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N22" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3215,22 +3629,22 @@
         <v>161</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J23" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="N23" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3259,22 +3673,22 @@
         <v>134</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J24" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="N24" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3303,22 +3717,22 @@
         <v>135</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J25" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="N25" s="2" t="s">
         <v>340</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="N25" s="2" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3326,43 +3740,43 @@
         <v>39</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="6">
+        <v>0</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0</v>
+      </c>
+      <c r="G26" s="6">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="E26" s="6">
-        <v>0</v>
-      </c>
-      <c r="F26" s="6">
-        <v>0</v>
-      </c>
-      <c r="G26" s="6">
-        <v>0</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>489</v>
-      </c>
       <c r="I26" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="J26" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="N26" s="2" t="s">
         <v>352</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3373,10 +3787,10 @@
         <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>490</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>491</v>
       </c>
       <c r="E27" s="6">
         <v>25</v>
@@ -3388,25 +3802,25 @@
         <v>20</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J27" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="N27" s="2" t="s">
         <v>358</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="N27" s="2" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3414,43 +3828,43 @@
         <v>41</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="6">
+        <v>0</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0</v>
+      </c>
+      <c r="G28" s="6">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="E28" s="6">
-        <v>0</v>
-      </c>
-      <c r="F28" s="6">
-        <v>0</v>
-      </c>
-      <c r="G28" s="6">
-        <v>0</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>496</v>
-      </c>
       <c r="I28" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J28" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="L28" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="K28" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="L28" s="2" t="s">
+      <c r="M28" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="N28" s="2" t="s">
         <v>365</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="N28" s="2" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3461,10 +3875,10 @@
         <v>10</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>497</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>498</v>
       </c>
       <c r="E29" s="6">
         <v>20</v>
@@ -3476,25 +3890,25 @@
         <v>15</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J29" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="N29" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3502,13 +3916,13 @@
         <v>43</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>501</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>502</v>
       </c>
       <c r="E30" s="6">
         <v>30</v>
@@ -3520,25 +3934,25 @@
         <v>25</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I30" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="N30" s="2" t="s">
         <v>377</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3546,13 +3960,13 @@
         <v>44</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>504</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>505</v>
       </c>
       <c r="E31" s="6">
         <v>30</v>
@@ -3564,25 +3978,25 @@
         <v>25</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J31" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="N31" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3590,43 +4004,43 @@
         <v>45</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="6">
+        <v>0</v>
+      </c>
+      <c r="F32" s="6">
+        <v>0</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="E32" s="6">
-        <v>0</v>
-      </c>
-      <c r="F32" s="6">
-        <v>0</v>
-      </c>
-      <c r="G32" s="6">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>510</v>
-      </c>
       <c r="I32" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="J32" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="K32" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="M32" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="K32" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="M32" s="2" t="s">
+      <c r="N32" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3634,13 +4048,13 @@
         <v>46</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>511</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>512</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>513</v>
       </c>
       <c r="E33" s="6">
         <v>25</v>
@@ -3652,25 +4066,25 @@
         <v>20</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I33" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="M33" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="N33" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="M33" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3699,22 +4113,22 @@
         <v>138</v>
       </c>
       <c r="I34" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="K34" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="L34" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="K34" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="L34" s="2" t="s">
+      <c r="M34" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="M34" s="2" t="s">
-        <v>403</v>
-      </c>
       <c r="N34" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3725,10 +4139,10 @@
         <v>21</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>515</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>516</v>
       </c>
       <c r="E35" s="6">
         <v>30</v>
@@ -3740,25 +4154,25 @@
         <v>25</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J35" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="N35" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="N35" s="2" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3769,40 +4183,40 @@
         <v>27</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="6">
+        <v>0</v>
+      </c>
+      <c r="F36" s="6">
+        <v>0</v>
+      </c>
+      <c r="G36" s="6">
+        <v>0</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="E36" s="6">
-        <v>0</v>
-      </c>
-      <c r="F36" s="6">
-        <v>0</v>
-      </c>
-      <c r="G36" s="6">
-        <v>0</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>520</v>
-      </c>
       <c r="I36" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="M36" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="J36" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>417</v>
-      </c>
       <c r="N36" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3813,40 +4227,40 @@
         <v>27</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="6">
+        <v>0</v>
+      </c>
+      <c r="F37" s="6">
+        <v>0</v>
+      </c>
+      <c r="G37" s="6">
+        <v>0</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="E37" s="6">
-        <v>0</v>
-      </c>
-      <c r="F37" s="6">
-        <v>0</v>
-      </c>
-      <c r="G37" s="6">
-        <v>0</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>523</v>
-      </c>
       <c r="I37" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="M37" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="J37" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>423</v>
-      </c>
       <c r="N37" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3857,7 +4271,7 @@
         <v>21</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>97</v>
@@ -3872,25 +4286,25 @@
         <v>30</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="J38" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="N38" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="N38" s="2" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3901,40 +4315,40 @@
         <v>27</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="6">
+        <v>0</v>
+      </c>
+      <c r="F39" s="6">
+        <v>0</v>
+      </c>
+      <c r="G39" s="6">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="E39" s="6">
-        <v>0</v>
-      </c>
-      <c r="F39" s="6">
-        <v>0</v>
-      </c>
-      <c r="G39" s="6">
-        <v>0</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>528</v>
-      </c>
       <c r="I39" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="M39" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="N39" s="2" t="s">
         <v>430</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="N39" s="2" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3945,40 +4359,40 @@
         <v>27</v>
       </c>
       <c r="C40" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="6">
+        <v>0</v>
+      </c>
+      <c r="F40" s="6">
+        <v>0</v>
+      </c>
+      <c r="G40" s="6">
+        <v>0</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="E40" s="6">
-        <v>0</v>
-      </c>
-      <c r="F40" s="6">
-        <v>0</v>
-      </c>
-      <c r="G40" s="6">
-        <v>0</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>531</v>
-      </c>
       <c r="I40" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="M40" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="J40" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>441</v>
-      </c>
       <c r="N40" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4006,8 +4420,23 @@
       <c r="H41" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>209</v>
+      <c r="I41" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4035,8 +4464,23 @@
       <c r="H42" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I42" s="2" t="s">
-        <v>209</v>
+      <c r="I42" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4064,8 +4508,23 @@
       <c r="H43" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I43" s="2" t="s">
-        <v>209</v>
+      <c r="I43" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4093,8 +4552,23 @@
       <c r="H44" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="I44" s="2" t="s">
-        <v>209</v>
+      <c r="I44" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4123,7 +4597,22 @@
         <v>128</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>209</v>
+        <v>559</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4151,8 +4640,23 @@
       <c r="H46" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I46" s="2" t="s">
-        <v>209</v>
+      <c r="I46" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4180,8 +4684,23 @@
       <c r="H47" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="I47" s="2" t="s">
-        <v>209</v>
+      <c r="I47" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4209,11 +4728,26 @@
       <c r="H48" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="I48" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I48" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="M48" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>64</v>
       </c>
@@ -4238,11 +4772,26 @@
       <c r="H49" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="I49" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I49" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>65</v>
       </c>
@@ -4267,11 +4816,26 @@
       <c r="H50" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="I50" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I50" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="N50" s="2" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>66</v>
       </c>
@@ -4296,11 +4860,26 @@
       <c r="H51" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="I51" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I51" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="N51" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>67</v>
       </c>
@@ -4325,11 +4904,26 @@
       <c r="H52" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="I52" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I52" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="N52" s="2" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>68</v>
       </c>
@@ -4354,11 +4948,26 @@
       <c r="H53" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="I53" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I53" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="N53" s="2" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>69</v>
       </c>
@@ -4383,11 +4992,26 @@
       <c r="H54" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="I54" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I54" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="N54" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>70</v>
       </c>
@@ -4412,11 +5036,26 @@
       <c r="H55" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="I55" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I55" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="N55" s="3" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>72</v>
       </c>
@@ -4441,11 +5080,26 @@
       <c r="H56" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="I56" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I56" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="N56" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>74</v>
       </c>
@@ -4470,11 +5124,26 @@
       <c r="H57" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="I57" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I57" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="N57" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>76</v>
       </c>
@@ -4499,11 +5168,26 @@
       <c r="H58" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="I58" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I58" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="N58" s="2" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>78</v>
       </c>
@@ -4528,11 +5212,26 @@
       <c r="H59" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="I59" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I59" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="N59" s="2" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>79</v>
       </c>
@@ -4557,11 +5256,26 @@
       <c r="H60" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="I60" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I60" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="N60" s="2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>80</v>
       </c>
@@ -4586,11 +5300,26 @@
       <c r="H61" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="I61" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I61" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="N61" s="2" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>81</v>
       </c>
@@ -4615,11 +5344,26 @@
       <c r="H62" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="I62" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I62" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="M62" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="N62" s="2" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>82</v>
       </c>
@@ -4645,10 +5389,25 @@
         <v>158</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+        <v>662</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="M63" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="N63" s="2" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>83</v>
       </c>
@@ -4673,8 +5432,23 @@
       <c r="H64" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="I64" s="2" t="s">
-        <v>209</v>
+      <c r="I64" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="N64" s="2" t="s">
+        <v>665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweaked formatting of Learn tab and hyperlinked all links
</commit_message>
<xml_diff>
--- a/Database - Learn.xlsx
+++ b/Database - Learn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GraceMaloney/Downloads/HCI 584X/Project/Code/National-Park-Journal-and-Learn_HCI584/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93017782-5B6C-B747-93AA-5806F3D1C24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC816308-E409-F54A-A319-87392053CE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{21CDAEF0-8EF3-284B-980A-1BFB33ABAC9E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="669">
   <si>
     <t>Name</t>
   </si>
@@ -408,9 +408,6 @@
   </si>
   <si>
     <t>Cost of Entry Per Motorcycle</t>
-  </si>
-  <si>
-    <t>$7 per person</t>
   </si>
   <si>
     <t>Location</t>
@@ -513,9 +510,6 @@
     </r>
   </si>
   <si>
-    <t>The highly glaciated mountains of the North Cascades Range exhibit a spectacular and complex geologic history. Between the river valleys and high peaks there are eight diverse life zones with 75 mammal and 1,600 vascular plant species. Popular hiking and climbing areas of the Stephen Mather Wilderness include Cascade Pass, Mount Shuksan, Mount Triumph, and Eldorado Peak. Ross Lake and Lake Chelan National Recreation Areas adjoin the two segments of the park and are all administered together.</t>
-  </si>
-  <si>
     <t>This park on the Olympic Peninsula includes a wide range of ecosystems from Pacific shoreline to temperate rainforests to the glaciated alpine peaks of the Olympic Mountains, the tallest of which is Mount Olympus. The Hoh and Quinault Rainforests are the wettest areas in the contiguous United States, with the Hoh receiving an average of almost 12 ft (3.7 m) of rain every year.</t>
   </si>
   <si>
@@ -526,9 +520,6 @@
   </si>
   <si>
     <t>This park and the co-managed state parks protect almost half of all remaining coastal redwoods, the tallest trees on earth. There are three large river systems in this very seismically active area, and 37 miles (60 km) of protected coastline reveal tide pools and seastacks. The prairie, estuary, coast, river, and forest ecosystems contain a wide variety of animal and plant species.</t>
-  </si>
-  <si>
-    <t>Bisected north to south by the Continental Divide, this portion of the Rockies has ecosystems varying from over 150 riparian lakes to montane and subalpine forests to treeless alpine tundra. Wildlife including elk, moose, mule deer, bighorn sheep, black bears, and cougars inhabit its igneous mountains and glacial valleys. Longs Peak, a classic Colorado fourteener, and the scenic Bear Lake are popular destinations, as well as the historic Trail Ridge Road, which reaches an elevation of more than 12,000 feet (3,700 m).</t>
   </si>
   <si>
     <t>Split into the separate Rincon Mountain and Tucson Mountain districts, this park is evidence that the dry Sonoran Desert is still home to a great variety of life spanning six biotic communities. Beyond the namesake giant saguaro cacti, there are barrel cacti, chollas, and prickly pears, as well as lesser long-nosed bats, spotted owls, and javelinas.</t>
@@ -601,9 +592,6 @@
     <t>The largest national park in the system protects the convergence of the Alaska, Chugach, Wrangell, and Saint Elias Ranges, which include many of the continent's tallest mountains and volcanoes, including the 18,008-foot Mount Saint Elias. More than a quarter of the park is covered with glaciers, including the tidewater Hubbard Glacier, piedmont Malaspina Glacier, and valley Nabesna Glacier.</t>
   </si>
   <si>
-    <t>Situated on the Yellowstone Caldera, the park has an expansive network of geothermal areas including boiling mud pots, vividly colored hot springs such as Grand Prismatic Spring, and regularly erupting geysers, the best-known being Old Faithful. The yellow-hued Grand Canyon of the Yellowstone River contains several high waterfalls, and four mountain ranges traverse the park. More than 60 mammal species including timber wolves, grizzly bears, black bears, lynxes, bison, and elk make this park one of the best wildlife viewing spots in the country.</t>
-  </si>
-  <si>
     <t>Yosemite features sheer granite cliffs, exceptionally tall waterfalls, and old-growth forests at a unique intersection of geology and hydrology. Half Dome and El Capitan rise from the park's centerpiece, the glacier-carved Yosemite Valley, and from its vertical walls drop Yosemite Falls, one of North America's tallest waterfalls at 2,425 feet (739 m) high. Three giant sequoia groves, along with a pristine wilderness in the heart of the Sierra Nevada, are home to a wide variety of rare plant and animal species.</t>
   </si>
   <si>
@@ -636,12 +624,6 @@
     </r>
   </si>
   <si>
-    <t>The U.S. half of Waterton-Glacier International Peace Park, this park includes 26 rapidly receding glaciers and 130 named lakes surrounded by Rocky Mountain peaks. Historic hotels and the landmark Going-to-the-Sun Road accommodate visitors. The local mountains, formed by an overthrust, expose Paleozoic fossils including trilobites, mollusks, giant ferns and dinosaurs. The park is also home to Triple Divide Peak, which forms the boundary between the watersheds of the Atlantic, Pacific, and Arctic Oceans.</t>
-  </si>
-  <si>
-    <t>Mount Rainier, an active stratovolcano, is the most prominent peak in the Cascades and is covered by 26 named glaciers including Carbon Glacier and Emmons Glacier, the longest and largest in the contiguous United States respectively. The mountain is popular for climbing, and more than half of the park is covered by subalpine and alpine forests and meadows seasonally in bloom with wildflowers. Paradise on the south slope is among the snowiest places on Earth. The Longmire visitor center is the start of the Wonderland Trail, which encircles the mountain.</t>
-  </si>
-  <si>
     <t>Wind Cave is distinctive for its calcite fin formations called boxwork, a unique formation rarely found elsewhere, and needle-like growths called frostwork. It is one of the longest caves in the world and creates a wind as air pressure changes. Above ground is a mixed-grass prairie with animals such as bison, black-footed ferrets, and prairie dogs and ponderosa pine forests home to cougars and elk. The cave is culturally significant to the Lakota people as a creation site.</t>
   </si>
   <si>
@@ -1572,9 +1554,6 @@
     <t>https://www.nps.gov/drto/index.htm</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>The islands of the Dry Tortugas, at the westernmost end of the Florida Keys, are the site of Fort Jefferson, a Civil War-era fort that is the largest masonry structure in the Western Hemisphere. The park is home to undisturbed coral reefs and shipwrecks, and is only accessible by plane or boat.</t>
   </si>
   <si>
@@ -1605,8 +1584,575 @@
     <t>https://www.nps.gov/jeff/index.htm</t>
   </si>
   <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>National Park Photos/Great Basin National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/grba/index.htm</t>
+  </si>
+  <si>
+    <t>Based around Nevada's second tallest mountain, Wheeler Peak, Great Basin National Park protects 5,000-year-old bristlecone pines, a rock glacier, and the limestone Lehman Caves. Due to its remote location, the park is home to some of the country's darkest night skies. Wildlife includes the Townsend's big-eared bat, pronghorn, and Bonneville cutthroat trout.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Great Sand Dunes National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/grsa/index.htm</t>
+  </si>
+  <si>
+    <t>The tallest sand dunes in North America, up to 750 feet (230 m) tall, were formed by deposits of the ancient Rio Grande in the San Luis Valley. Abutting a variety of grasslands, shrublands, and wetlands, the park also features alpine lakes, six 13,000-foot mountains, and old-growth forests.</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>National Park Photos/Great Smoky Mountains National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/grsm/index.htm</t>
+  </si>
+  <si>
+    <t>The Great Smoky Mountains, part of the Appalachian Mountains, span a wide range of elevations, making them home to over 400 vertebrate species, 100 tree species, and 5,000 plant species. Hiking is the park's main attraction, with over 800 miles (1,300 km) of trails, including 70 miles (110 km) of the Appalachian Trail. Other activities include fishing, horseback riding, and touring nearly 80 historic structures.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Guadalupe Mountains National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/gumo/index.htm</t>
+  </si>
+  <si>
+    <t>This park contains Guadalupe Peak, the highest point in Texas, as well as the scenic McKittrick Canyon filled with bigtooth maples, a corner of the arid Chihuahuan Desert, and a fossilized coral reef from the Permian era.</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>National Park Photos/Haleakala National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/hale/index.htm</t>
+  </si>
+  <si>
+    <t>The Haleakalā volcano on Maui features a very large crater with numerous cinder cones, a grove of non-native trees, the Kipahulu section's scenic pools of freshwater fish, and the endemic Hawaiian goose. The park protects the greatest number of endangered species within a U.S. national park.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Hawai’i Volcanoes National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/havo/index.htm</t>
+  </si>
+  <si>
+    <t>This park on the Big Island protects the Kīlauea and Mauna Loa volcanoes, two of the world's most active geological features. Diverse ecosystems range from tropical forests at sea level to barren lava beds at more than 13,000 feet (4,000 m).</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>National Park Photos/Hot Springs National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/hosp/index.htm</t>
+  </si>
+  <si>
+    <t>Hot Springs was originally established by Congress as a federal reserve on April 20, 1832, making it the oldest area managed by the National Park Service. Natural thermal springs flow out of the Ouachita Mountains, providing opportunities for relaxation in a historic setting. Bathhouse Row preserves examples of 19th-century architecture. Hot Springs is the first national park within a city and was the smallest national park until 2018.</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>National Park Photos/Indiana Dunes National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/indu/index.htm</t>
+  </si>
+  <si>
+    <t>Previously designated a national lakeshore, parts of this 20-mile (32 km) stretch of the southern shore of Lake Michigan have sandy beaches and tall dunes. The park includes grassy prairies, peat bogs, and marsh wetlands home to over 2,000 species.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Joshua Tree National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/jotr/index.htm</t>
+  </si>
+  <si>
+    <t>Covering large areas of the Colorado and Mojave Deserts and the Little San Bernardino Mountains, this desert landscape is populated by vast stands of Joshua trees. Large changes in elevation reveal various contrasting environments including bleached sand dunes, dry lakes, rugged mountains, and maze-like clusters of monzogranite monoliths.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Katmai National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/katm/index.htm</t>
+  </si>
+  <si>
+    <t>This park on the Alaska Peninsula protects the Valley of Ten Thousand Smokes, an ash flow formed by the 1912 eruption of Novarupta, and the stratovolcano Mount Katmai. Over 2,000 grizzly bears come here each year to catch spawning salmon. Other wildlife includes caribou, wolves, moose, and wolverines.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Kenai Fjords National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/kefj/index.htm</t>
+  </si>
+  <si>
+    <t>Near Seward on the Kenai Peninsula, this park protects the Harding Icefield and at least 38 glaciers and fjords stemming from it. The only area accessible to the public by road is the rapidly shrinking Exit Glacier. Boat and kayak tours offer views of tidewater glaciers, whales, sea lions, and marine birds.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Kings Canyon National Park.jpg</t>
+  </si>
+  <si>
+    <t>Home to several giant sequoia groves and the General Grant Tree, the world's second largest measured tree, this park also features part of the Kings River, sculptor of the dramatic granite canyon that is its namesake, and the San Joaquin River, as well as Boyden Cave. Although Kings Canyon National Park was designated as such in 1940, it subsumed General Grant National Park, which had been established on October 1, 1890, as the United States' fourth national park.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Kobuk Valley National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/kova/index.htm</t>
+  </si>
+  <si>
+    <t>Kobuk Valley protects 61 miles (98 km) of the Kobuk River and three regions of sand dunes. Created by glaciers, the Great Kobuk, Little Kobuk, and Hunt River Sand Dunes can reach 100 feet (30 m) high and 100 °F (38 °C), and they are the largest dunes in the Arctic. Twice a year, half a million caribou migrate through the dunes and across river bluffs that expose well-preserved ice age fossils.</t>
+  </si>
+  <si>
+    <t>National Park Photos/Lake Clark National Park.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/lacl/index.htm</t>
+  </si>
+  <si>
+    <t>The region around Lake Clark features four active volcanoes, including Mount Redoubt, as well as an abundance of rivers, glaciers, and waterfalls. Temperate rainforests, a tundra plateau, and three mountain ranges complete the landscape.</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/lavo/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/lavo/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/lavo/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Black bears, sierra neveda red foxes, moutain lions, pikas, otters</t>
+  </si>
+  <si>
+    <t>Hiking, backpacking, biking, kayaking, fishing, swimming</t>
+  </si>
+  <si>
+    <t>Lassen Volcanic National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/maca/planyourvisit/operatinghoursandseasons.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/maca/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/maca/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Bats, skinks, bullfrogs, turtles</t>
+  </si>
+  <si>
+    <t>Cave touring, biking, hiking, kayaking, canoeing, fishing</t>
+  </si>
+  <si>
+    <t>Mammoth Cave National Park is open year-round.</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/meve/planyourvisit/basicinfo.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/meve/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/meve/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Mexican spotted owls, elk, black bears, bats, rattlesnakes, weasels</t>
+  </si>
+  <si>
+    <t>Hiking, camping, cliff dwelling tours</t>
+  </si>
+  <si>
+    <t>Mesa Verde National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Mount Rainier National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/mora/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/mora/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/mora/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Black bears, cascade red foxes, moutain lions, elk, mountain goats, moose</t>
+  </si>
+  <si>
+    <t>Hiking, camping, rock climbing, biking, fishing, mountaineering</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/npsa/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/npsa/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/npsa/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Humpback whales, sperm whales, orcas, dolphins, sea turtles, geckos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The National Park of American Samoa is open year-round, but some areas of the park may be temporarily closed due to trail maintenance or safety measures.</t>
+  </si>
+  <si>
+    <t>Fishing, snorkeling, hiking, diving, beachwalking</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/neri/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/neri/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/neri/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Whitewater rafting, hiking, camping, biking, rock climbing, fishing</t>
+  </si>
+  <si>
+    <t>Black bears, red foxes, beavers, minks, river otters</t>
+  </si>
+  <si>
+    <t>New River Gorge National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/noca/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/noca/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/noca/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Mountain goats, bighorn sheep, elk, moose, gray wolves, red foxes, river otters</t>
+  </si>
+  <si>
+    <t>Hiking, backpacking, camping, canoeing, kayaking, biking, mountaineering</t>
+  </si>
+  <si>
+    <t>North Cascades National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/olym/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/olym/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/olym/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Whales, dolphins, sea lions, seals, sea otters, elk, black bears</t>
+  </si>
+  <si>
+    <t>Kayaking, fishing, camping, hiking, backpacking, climbing, skiing</t>
+  </si>
+  <si>
+    <t>Olympic National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/pefo/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/pefo/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/pefo/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Kit foxes, coyote, pronghorn, badgers, bobcats</t>
+  </si>
+  <si>
+    <t>Petrified Forest National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Hiking, backpacking, camping, biking, geocaching</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/pinn/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/pinn/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/pinn/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Canyon bats, mountain lions, condors, foxes, badgers, bobcats</t>
+  </si>
+  <si>
+    <t>Hiking, camping, rock climbing, bird watching</t>
+  </si>
+  <si>
+    <t>Pinnacles National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/redw/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/redw/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/redw/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Elk, mountain beavers, mountain lions, black bears, gray whales, sea lions, elephant seals, orcas, humpback whales, condors</t>
+  </si>
+  <si>
+    <t>Biking, hiking, camping, kayaking</t>
+  </si>
+  <si>
+    <t>Redwood National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/romo/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/romo/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/romo/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Hiking, camping, backpacking, scenic driving, fishing</t>
+  </si>
+  <si>
+    <t>Bighorn sheep, moose, black bears, mountain lions, elk, beavers</t>
+  </si>
+  <si>
+    <t>Rocky Mountain National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/sagu/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/sagu/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/sagu/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Bobcats, packrats, gray foxes, mountain lions, javelinas</t>
+  </si>
+  <si>
+    <t>Camping, hiking, biking</t>
+  </si>
+  <si>
+    <t>Saguaro National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Sequoia National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/shen/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/shen/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Black bears, bobcats, bats, deer, shrews</t>
+  </si>
+  <si>
+    <t>Shenandoah National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/shen/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>Hiking, backcountry camping, scenic driving, fishing, biking</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/thro/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/thro/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/thro/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Bison, wild horses, elk, deer, pronghorn, prairie dogs</t>
+  </si>
+  <si>
+    <t>Theodore Roosevelt National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Scenic driving, hiking, camping</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/viis/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/viis/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/viis/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Sea turtles, nurse sharks, whale sharks, stingrays</t>
+  </si>
+  <si>
+    <t>Virgin Islands National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Snorkeling, swimming, fishing, hiking, boating</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/voya/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/voya/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/voya/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Moose, beavers, wolves, otters, sturgeon, bears</t>
+  </si>
+  <si>
+    <t>Voyageurs National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Canoeing, hiking, boating, snowshoeing, cross-country skiing, fishing, camping</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/whsa/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/whsa/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/whsa/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Badgers, apache pocket mice, bobcats, kit foxes, bats, gophers</t>
+  </si>
+  <si>
+    <t>White Sands National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Sledding, hiking, biking, backcountry camping, dune driving</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/wica/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/wica/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/wica/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Bison, prairie dogs, ferrets, elk, pronghorn</t>
+  </si>
+  <si>
+    <t>Hiking, cave exploring, cave tours</t>
+  </si>
+  <si>
+    <t>Wind Cave National Park is open year-round</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/wrst/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/wrst/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Polar bears, moose, mountain goats, caribou, black bears, grizzly/brown bears, sea lions</t>
+  </si>
+  <si>
+    <t>Backpacking, mountaineering, boating, fishing, hiking, cross-country skiing</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/wrst/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>Wrangell St. Elias National Park is open year-round, with visitation most popular from May through September</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/yell/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/yell/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/yell/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Black bears, bobcats, lynx, badgers, gray wolves, grizzly bears, foxes, river otters</t>
+  </si>
+  <si>
+    <t>Hiking, camping, biking, scenic driving, cross-country skiing, snowshoeing</t>
+  </si>
+  <si>
+    <t>Yellowstone National Park is open year-round, but facilities are limited or closed during winter months</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/yose/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/yose/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/yose/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Black bears, bighorn sheep, red foxes, pacific fishers, mountain lions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yosemite National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Camping, hiking, backpacking, biking, fishing, rock climbing, swimming, kayaking</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/zion/planyourvisit/hours.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/zion/planyourvisit/things2do.htm</t>
+  </si>
+  <si>
+    <t>https://www.nps.gov/zion/learn/nature/index.htm</t>
+  </si>
+  <si>
+    <t>Foxes, black bears, ringtail, badgers, mountain lions, elk, bighorn sheep</t>
+  </si>
+  <si>
+    <t>Backpacking, hiking, river hiking, camping, canyoneering, rock climbing, kayaking, biking</t>
+  </si>
+  <si>
+    <t>Zion National Park is open year-round</t>
+  </si>
+  <si>
+    <t>Situated on the Yellowstone Caldera, the park has an expansive network of geothermal areas including boiling mud pots, vividly colored hot springs such as Grand Prismatic Spring, and regularly erupting geysers, the best-known being Old Faithful. The yellow-hued Grand Canyon of the Yellowstone River contains several high waterfalls, and four mountain ranges traverse the park.</t>
+  </si>
+  <si>
+    <t>7 per person</t>
+  </si>
+  <si>
+    <t>Mount Rainier, an active stratovolcano, is the most prominent peak in the Cascades and is covered by 26 named glaciers including Carbon Glacier and Emmons Glacier, the longest and largest in the contiguous United States respectively. The mountain is popular for climbing, and more than half of the park is covered by subalpine and alpine forests and meadows seasonally in bloom with wildflowers. Paradise on the south slope is among the snowiest places on Earth.</t>
+  </si>
+  <si>
+    <t>Bisected north to south by the Continental Divide, this portion of the Rockies has ecosystems varying from over 150 riparian lakes to montane and subalpine forests to treeless alpine tundra. Wildlife inhabit its igneous mountains and glacial valleys. Longs Peak, a classic Colorado fourteener, and the scenic Bear Lake are popular destinations, as well as the historic Trail Ridge Road, which reaches an elevation of more than 12,000 feet (3,700 m).</t>
+  </si>
+  <si>
     <r>
-      <t>The Gateway Arch is a 630-foot (192 m) (both high and wide) catenary arch built in the 1960s to commemorate the Lewis and Clark Expedition, initiated by Thomas Jefferson, and the subsequent westward expansion of the country. The nearby Old Courthouse, across a greenway to the west of the arch, was the original site of the landmark </t>
+      <t>The Gateway Arch is a 630-foot catenary arch built in the 1960s to commemorate the Lewis and Clark Expedition, initiated by Thomas Jefferson, and the subsequent westward expansion of the country. The nearby Old Courthouse, across a greenway to the west of the arch, was the original site of the landmark </t>
     </r>
     <r>
       <rPr>
@@ -1631,559 +2177,10 @@
     </r>
   </si>
   <si>
-    <t>Nevada</t>
-  </si>
-  <si>
-    <t>National Park Photos/Great Basin National Park.jpg</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/grba/index.htm</t>
-  </si>
-  <si>
-    <t>Based around Nevada's second tallest mountain, Wheeler Peak, Great Basin National Park protects 5,000-year-old bristlecone pines, a rock glacier, and the limestone Lehman Caves. Due to its remote location, the park is home to some of the country's darkest night skies. Wildlife includes the Townsend's big-eared bat, pronghorn, and Bonneville cutthroat trout.</t>
-  </si>
-  <si>
-    <t>National Park Photos/Great Sand Dunes National Park.jpg</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/grsa/index.htm</t>
-  </si>
-  <si>
-    <t>The tallest sand dunes in North America, up to 750 feet (230 m) tall, were formed by deposits of the ancient Rio Grande in the San Luis Valley. Abutting a variety of grasslands, shrublands, and wetlands, the park also features alpine lakes, six 13,000-foot mountains, and old-growth forests.</t>
-  </si>
-  <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
-    <t>National Park Photos/Great Smoky Mountains National Park.jpg</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/grsm/index.htm</t>
-  </si>
-  <si>
-    <t>The Great Smoky Mountains, part of the Appalachian Mountains, span a wide range of elevations, making them home to over 400 vertebrate species, 100 tree species, and 5,000 plant species. Hiking is the park's main attraction, with over 800 miles (1,300 km) of trails, including 70 miles (110 km) of the Appalachian Trail. Other activities include fishing, horseback riding, and touring nearly 80 historic structures.</t>
-  </si>
-  <si>
-    <t>National Park Photos/Guadalupe Mountains National Park.jpg</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/gumo/index.htm</t>
-  </si>
-  <si>
-    <t>This park contains Guadalupe Peak, the highest point in Texas, as well as the scenic McKittrick Canyon filled with bigtooth maples, a corner of the arid Chihuahuan Desert, and a fossilized coral reef from the Permian era.</t>
-  </si>
-  <si>
-    <t>Hawaii</t>
-  </si>
-  <si>
-    <t>National Park Photos/Haleakala National Park.jpg</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/hale/index.htm</t>
-  </si>
-  <si>
-    <t>The Haleakalā volcano on Maui features a very large crater with numerous cinder cones, a grove of non-native trees, the Kipahulu section's scenic pools of freshwater fish, and the endemic Hawaiian goose. The park protects the greatest number of endangered species within a U.S. national park.</t>
-  </si>
-  <si>
-    <t>National Park Photos/Hawai’i Volcanoes National Park.jpg</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/havo/index.htm</t>
-  </si>
-  <si>
-    <t>This park on the Big Island protects the Kīlauea and Mauna Loa volcanoes, two of the world's most active geological features. Diverse ecosystems range from tropical forests at sea level to barren lava beds at more than 13,000 feet (4,000 m).</t>
-  </si>
-  <si>
-    <t>Arkansas</t>
-  </si>
-  <si>
-    <t>National Park Photos/Hot Springs National Park.jpg</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/hosp/index.htm</t>
-  </si>
-  <si>
-    <t>Hot Springs was originally established by Congress as a federal reserve on April 20, 1832, making it the oldest area managed by the National Park Service. Natural thermal springs flow out of the Ouachita Mountains, providing opportunities for relaxation in a historic setting. Bathhouse Row preserves examples of 19th-century architecture. Hot Springs is the first national park within a city and was the smallest national park until 2018.</t>
-  </si>
-  <si>
-    <t>Indiana</t>
-  </si>
-  <si>
-    <t>National Park Photos/Indiana Dunes National Park.jpg</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/indu/index.htm</t>
-  </si>
-  <si>
-    <t>Previously designated a national lakeshore, parts of this 20-mile (32 km) stretch of the southern shore of Lake Michigan have sandy beaches and tall dunes. The park includes grassy prairies, peat bogs, and marsh wetlands home to over 2,000 species.</t>
-  </si>
-  <si>
-    <t>National Park Photos/Joshua Tree National Park.jpg</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/jotr/index.htm</t>
-  </si>
-  <si>
-    <t>Covering large areas of the Colorado and Mojave Deserts and the Little San Bernardino Mountains, this desert landscape is populated by vast stands of Joshua trees. Large changes in elevation reveal various contrasting environments including bleached sand dunes, dry lakes, rugged mountains, and maze-like clusters of monzogranite monoliths.</t>
-  </si>
-  <si>
-    <t>National Park Photos/Katmai National Park.jpg</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/katm/index.htm</t>
-  </si>
-  <si>
-    <t>This park on the Alaska Peninsula protects the Valley of Ten Thousand Smokes, an ash flow formed by the 1912 eruption of Novarupta, and the stratovolcano Mount Katmai. Over 2,000 grizzly bears come here each year to catch spawning salmon. Other wildlife includes caribou, wolves, moose, and wolverines.</t>
-  </si>
-  <si>
-    <t>National Park Photos/Kenai Fjords National Park.jpg</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/kefj/index.htm</t>
-  </si>
-  <si>
-    <t>Near Seward on the Kenai Peninsula, this park protects the Harding Icefield and at least 38 glaciers and fjords stemming from it. The only area accessible to the public by road is the rapidly shrinking Exit Glacier. Boat and kayak tours offer views of tidewater glaciers, whales, sea lions, and marine birds.</t>
-  </si>
-  <si>
-    <t>National Park Photos/Kings Canyon National Park.jpg</t>
-  </si>
-  <si>
-    <t>Home to several giant sequoia groves and the General Grant Tree, the world's second largest measured tree, this park also features part of the Kings River, sculptor of the dramatic granite canyon that is its namesake, and the San Joaquin River, as well as Boyden Cave. Although Kings Canyon National Park was designated as such in 1940, it subsumed General Grant National Park, which had been established on October 1, 1890, as the United States' fourth national park.</t>
-  </si>
-  <si>
-    <t>National Park Photos/Kobuk Valley National Park.jpg</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/kova/index.htm</t>
-  </si>
-  <si>
-    <t>Kobuk Valley protects 61 miles (98 km) of the Kobuk River and three regions of sand dunes. Created by glaciers, the Great Kobuk, Little Kobuk, and Hunt River Sand Dunes can reach 100 feet (30 m) high and 100 °F (38 °C), and they are the largest dunes in the Arctic. Twice a year, half a million caribou migrate through the dunes and across river bluffs that expose well-preserved ice age fossils.</t>
-  </si>
-  <si>
-    <t>National Park Photos/Lake Clark National Park.jpg</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/lacl/index.htm</t>
-  </si>
-  <si>
-    <t>The region around Lake Clark features four active volcanoes, including Mount Redoubt, as well as an abundance of rivers, glaciers, and waterfalls. Temperate rainforests, a tundra plateau, and three mountain ranges complete the landscape.</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/lavo/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/lavo/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/lavo/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Black bears, sierra neveda red foxes, moutain lions, pikas, otters</t>
-  </si>
-  <si>
-    <t>Hiking, backpacking, biking, kayaking, fishing, swimming</t>
-  </si>
-  <si>
-    <t>Lassen Volcanic National Park is open year-round</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/maca/planyourvisit/operatinghoursandseasons.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/maca/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/maca/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Bats, skinks, bullfrogs, turtles</t>
-  </si>
-  <si>
-    <t>Cave touring, biking, hiking, kayaking, canoeing, fishing</t>
-  </si>
-  <si>
-    <t>Mammoth Cave National Park is open year-round.</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/meve/planyourvisit/basicinfo.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/meve/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/meve/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Mexican spotted owls, elk, black bears, bats, rattlesnakes, weasels</t>
-  </si>
-  <si>
-    <t>Hiking, camping, cliff dwelling tours</t>
-  </si>
-  <si>
-    <t>Mesa Verde National Park is open year-round</t>
-  </si>
-  <si>
-    <t>Mount Rainier National Park is open year-round</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/mora/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/mora/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/mora/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Black bears, cascade red foxes, moutain lions, elk, mountain goats, moose</t>
-  </si>
-  <si>
-    <t>Hiking, camping, rock climbing, biking, fishing, mountaineering</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/npsa/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/npsa/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/npsa/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Humpback whales, sperm whales, orcas, dolphins, sea turtles, geckos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The National Park of American Samoa is open year-round, but some areas of the park may be temporarily closed due to trail maintenance or safety measures.</t>
-  </si>
-  <si>
-    <t>Fishing, snorkeling, hiking, diving, beachwalking</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/neri/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/neri/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/neri/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Whitewater rafting, hiking, camping, biking, rock climbing, fishing</t>
-  </si>
-  <si>
-    <t>Black bears, red foxes, beavers, minks, river otters</t>
-  </si>
-  <si>
-    <t>New River Gorge National Park is open year-round</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/noca/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/noca/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/noca/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Mountain goats, bighorn sheep, elk, moose, gray wolves, red foxes, river otters</t>
-  </si>
-  <si>
-    <t>Hiking, backpacking, camping, canoeing, kayaking, biking, mountaineering</t>
-  </si>
-  <si>
-    <t>North Cascades National Park is open year-round</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/olym/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/olym/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/olym/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Whales, dolphins, sea lions, seals, sea otters, elk, black bears</t>
-  </si>
-  <si>
-    <t>Kayaking, fishing, camping, hiking, backpacking, climbing, skiing</t>
-  </si>
-  <si>
-    <t>Olympic National Park is open year-round</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/pefo/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/pefo/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/pefo/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Kit foxes, coyote, pronghorn, badgers, bobcats</t>
-  </si>
-  <si>
-    <t>Petrified Forest National Park is open year-round</t>
-  </si>
-  <si>
-    <t>Hiking, backpacking, camping, biking, geocaching</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/pinn/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/pinn/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/pinn/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Canyon bats, mountain lions, condors, foxes, badgers, bobcats</t>
-  </si>
-  <si>
-    <t>Hiking, camping, rock climbing, bird watching</t>
-  </si>
-  <si>
-    <t>Pinnacles National Park is open year-round</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/redw/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/redw/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/redw/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Elk, mountain beavers, mountain lions, black bears, gray whales, sea lions, elephant seals, orcas, humpback whales, condors</t>
-  </si>
-  <si>
-    <t>Biking, hiking, camping, kayaking</t>
-  </si>
-  <si>
-    <t>Redwood National Park is open year-round</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/romo/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/romo/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/romo/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Hiking, camping, backpacking, scenic driving, fishing</t>
-  </si>
-  <si>
-    <t>Bighorn sheep, moose, black bears, mountain lions, elk, beavers</t>
-  </si>
-  <si>
-    <t>Rocky Mountain National Park is open year-round</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/sagu/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/sagu/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/sagu/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Bobcats, packrats, gray foxes, mountain lions, javelinas</t>
-  </si>
-  <si>
-    <t>Camping, hiking, biking</t>
-  </si>
-  <si>
-    <t>Saguaro National Park is open year-round</t>
-  </si>
-  <si>
-    <t>Sequoia National Park is open year-round</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/shen/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/shen/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Black bears, bobcats, bats, deer, shrews</t>
-  </si>
-  <si>
-    <t>Shenandoah National Park is open year-round</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/shen/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>Hiking, backcountry camping, scenic driving, fishing, biking</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/thro/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/thro/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/thro/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Bison, wild horses, elk, deer, pronghorn, prairie dogs</t>
-  </si>
-  <si>
-    <t>Theodore Roosevelt National Park is open year-round</t>
-  </si>
-  <si>
-    <t>Scenic driving, hiking, camping</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/viis/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/viis/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/viis/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Sea turtles, nurse sharks, whale sharks, stingrays</t>
-  </si>
-  <si>
-    <t>Virgin Islands National Park is open year-round</t>
-  </si>
-  <si>
-    <t>Snorkeling, swimming, fishing, hiking, boating</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/voya/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/voya/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/voya/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Moose, beavers, wolves, otters, sturgeon, bears</t>
-  </si>
-  <si>
-    <t>Voyageurs National Park is open year-round</t>
-  </si>
-  <si>
-    <t>Canoeing, hiking, boating, snowshoeing, cross-country skiing, fishing, camping</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/whsa/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/whsa/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/whsa/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Badgers, apache pocket mice, bobcats, kit foxes, bats, gophers</t>
-  </si>
-  <si>
-    <t>White Sands National Park is open year-round</t>
-  </si>
-  <si>
-    <t>Sledding, hiking, biking, backcountry camping, dune driving</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/wica/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/wica/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/wica/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Bison, prairie dogs, ferrets, elk, pronghorn</t>
-  </si>
-  <si>
-    <t>Hiking, cave exploring, cave tours</t>
-  </si>
-  <si>
-    <t>Wind Cave National Park is open year-round</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/wrst/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/wrst/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Polar bears, moose, mountain goats, caribou, black bears, grizzly/brown bears, sea lions</t>
-  </si>
-  <si>
-    <t>Backpacking, mountaineering, boating, fishing, hiking, cross-country skiing</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/wrst/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>Wrangell St. Elias National Park is open year-round, with visitation most popular from May through September</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/yell/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/yell/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/yell/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Black bears, bobcats, lynx, badgers, gray wolves, grizzly bears, foxes, river otters</t>
-  </si>
-  <si>
-    <t>Hiking, camping, biking, scenic driving, cross-country skiing, snowshoeing</t>
-  </si>
-  <si>
-    <t>Yellowstone National Park is open year-round, but facilities are limited or closed during winter months</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/yose/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/yose/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/yose/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Black bears, bighorn sheep, red foxes, pacific fishers, mountain lions</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Yosemite National Park is open year-round</t>
-  </si>
-  <si>
-    <t>Camping, hiking, backpacking, biking, fishing, rock climbing, swimming, kayaking</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/zion/planyourvisit/hours.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/zion/planyourvisit/things2do.htm</t>
-  </si>
-  <si>
-    <t>https://www.nps.gov/zion/learn/nature/index.htm</t>
-  </si>
-  <si>
-    <t>Foxes, black bears, ringtail, badgers, mountain lions, elk, bighorn sheep</t>
-  </si>
-  <si>
-    <t>Backpacking, hiking, river hiking, camping, canyoneering, rock climbing, kayaking, biking</t>
-  </si>
-  <si>
-    <t>Zion National Park is open year-round</t>
+    <t>The U.S. half of Waterton-Glacier International Peace Park, this park includes 26 rapidly receding glaciers and 130 named lakes surrounded by Rocky Mountain peaks. The local mountains, formed by an overthrust, expose Paleozoic fossils including trilobites, mollusks, giant ferns and dinosaurs. The park is also home to Triple Divide Peak, which forms the boundary between the watersheds of the Atlantic, Pacific, and Arctic Oceans.</t>
+  </si>
+  <si>
+    <t>The glaciated mountains of the North Cascades Range exhibit a spectacular geologic history. Between the river valleys and high peaks, there are 8 diverse life zones with 75 mammals and 1,600 plant species. Popular hiking and climbing areas of the Stephen Mather Wilderness include Cascade Pass, Mount Shuksan, Mount Triumph, and Eldorado Peak. Ross Lake and Lake Chelan National Recreation Areas adjoin the two segments of the park.</t>
   </si>
 </sst>
 </file>
@@ -2612,8 +2609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC95574-44B1-8347-90F2-3758EB862849}">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2640,13 +2637,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>121</v>
@@ -2658,25 +2655,25 @@
         <v>123</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2687,7 +2684,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>85</v>
@@ -2702,25 +2699,25 @@
         <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2731,7 +2728,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>86</v>
@@ -2746,25 +2743,25 @@
         <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2775,7 +2772,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>87</v>
@@ -2790,25 +2787,25 @@
         <v>25</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2819,7 +2816,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>88</v>
@@ -2834,25 +2831,25 @@
         <v>25</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2863,7 +2860,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>89</v>
@@ -2878,25 +2875,25 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2907,7 +2904,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>90</v>
@@ -2922,25 +2919,25 @@
         <v>25</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2951,10 +2948,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="E8" s="6">
         <v>35</v>
@@ -2966,25 +2963,25 @@
         <v>30</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2995,10 +2992,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="E9" s="6">
         <v>30</v>
@@ -3010,25 +3007,25 @@
         <v>25</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3039,10 +3036,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="E10" s="6">
         <v>20</v>
@@ -3054,25 +3051,25 @@
         <v>15</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3083,10 +3080,10 @@
         <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="E11" s="6">
         <v>30</v>
@@ -3098,25 +3095,25 @@
         <v>25</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3127,10 +3124,10 @@
         <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="E12" s="6">
         <v>0</v>
@@ -3142,25 +3139,25 @@
         <v>0</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3168,13 +3165,13 @@
         <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="E13" s="6">
         <v>0</v>
@@ -3186,25 +3183,25 @@
         <v>0</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3212,13 +3209,13 @@
         <v>23</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="E14" s="6">
         <v>30</v>
@@ -3230,25 +3227,25 @@
         <v>25</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3256,13 +3253,13 @@
         <v>24</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="E15" s="6">
         <v>0</v>
@@ -3274,25 +3271,25 @@
         <v>0</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3303,10 +3300,10 @@
         <v>21</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="E16" s="6">
         <v>30</v>
@@ -3318,25 +3315,25 @@
         <v>25</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3347,7 +3344,7 @@
         <v>27</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>91</v>
@@ -3362,25 +3359,25 @@
         <v>25</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="J17" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>209</v>
-      </c>
       <c r="M17" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3391,40 +3388,40 @@
         <v>12</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>473</v>
+        <v>466</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0</v>
       </c>
       <c r="F18" s="6">
         <v>15</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>473</v>
+      <c r="G18" s="6">
+        <v>0</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3435,10 +3432,10 @@
         <v>12</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="E19" s="6">
         <v>30</v>
@@ -3450,25 +3447,25 @@
         <v>25</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3479,10 +3476,10 @@
         <v>27</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="E20" s="6">
         <v>0</v>
@@ -3494,25 +3491,25 @@
         <v>0</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3520,13 +3517,13 @@
         <v>31</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="E21" s="6">
         <v>0</v>
@@ -3538,25 +3535,25 @@
         <v>0</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>484</v>
+        <v>666</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3567,7 +3564,7 @@
         <v>27</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>92</v>
@@ -3582,25 +3579,25 @@
         <v>0</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3611,7 +3608,7 @@
         <v>33</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>93</v>
@@ -3626,25 +3623,25 @@
         <v>30</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>161</v>
+        <v>667</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3655,7 +3652,7 @@
         <v>36</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>94</v>
@@ -3670,25 +3667,25 @@
         <v>30</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3699,7 +3696,7 @@
         <v>38</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>95</v>
@@ -3714,25 +3711,25 @@
         <v>30</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3740,13 +3737,13 @@
         <v>39</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="E26" s="6">
         <v>0</v>
@@ -3758,25 +3755,25 @@
         <v>0</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3787,10 +3784,10 @@
         <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="E27" s="6">
         <v>25</v>
@@ -3802,25 +3799,25 @@
         <v>20</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3828,13 +3825,13 @@
         <v>41</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="E28" s="6">
         <v>0</v>
@@ -3846,25 +3843,25 @@
         <v>0</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3875,10 +3872,10 @@
         <v>10</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="E29" s="6">
         <v>20</v>
@@ -3890,25 +3887,25 @@
         <v>15</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3916,13 +3913,13 @@
         <v>43</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="E30" s="6">
         <v>30</v>
@@ -3934,25 +3931,25 @@
         <v>25</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -3960,13 +3957,13 @@
         <v>44</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="E31" s="6">
         <v>30</v>
@@ -3978,25 +3975,25 @@
         <v>25</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4004,13 +4001,13 @@
         <v>45</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="E32" s="6">
         <v>0</v>
@@ -4022,25 +4019,25 @@
         <v>0</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4048,13 +4045,13 @@
         <v>46</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="E33" s="6">
         <v>25</v>
@@ -4066,25 +4063,25 @@
         <v>20</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4095,40 +4092,40 @@
         <v>84</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>96</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>124</v>
+        <v>663</v>
       </c>
       <c r="F34" s="6">
         <v>7</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>124</v>
+        <v>663</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4139,10 +4136,10 @@
         <v>21</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="E35" s="6">
         <v>30</v>
@@ -4154,25 +4151,25 @@
         <v>25</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4183,10 +4180,10 @@
         <v>27</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="E36" s="6">
         <v>0</v>
@@ -4198,25 +4195,25 @@
         <v>0</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4227,10 +4224,10 @@
         <v>27</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="E37" s="6">
         <v>0</v>
@@ -4242,25 +4239,25 @@
         <v>0</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4271,7 +4268,7 @@
         <v>21</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>97</v>
@@ -4286,25 +4283,25 @@
         <v>30</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4315,10 +4312,10 @@
         <v>27</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="E39" s="6">
         <v>0</v>
@@ -4330,25 +4327,25 @@
         <v>0</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4359,10 +4356,10 @@
         <v>27</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="E40" s="6">
         <v>0</v>
@@ -4374,25 +4371,25 @@
         <v>0</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4403,7 +4400,7 @@
         <v>21</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>98</v>
@@ -4418,25 +4415,25 @@
         <v>25</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4447,7 +4444,7 @@
         <v>56</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>99</v>
@@ -4462,25 +4459,25 @@
         <v>0</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4491,7 +4488,7 @@
         <v>14</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>100</v>
@@ -4506,25 +4503,25 @@
         <v>25</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4535,7 +4532,7 @@
         <v>59</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>101</v>
@@ -4550,25 +4547,25 @@
         <v>25</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>162</v>
+        <v>664</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4579,7 +4576,7 @@
         <v>6</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>102</v>
@@ -4594,25 +4591,25 @@
         <v>0</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4623,7 +4620,7 @@
         <v>61</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>103</v>
@@ -4638,25 +4635,25 @@
         <v>0</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4667,7 +4664,7 @@
         <v>59</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>104</v>
@@ -4682,25 +4679,25 @@
         <v>0</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>143</v>
+        <v>668</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4711,7 +4708,7 @@
         <v>59</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>105</v>
@@ -4726,25 +4723,25 @@
         <v>25</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4755,7 +4752,7 @@
         <v>36</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>106</v>
@@ -4770,25 +4767,25 @@
         <v>20</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4799,7 +4796,7 @@
         <v>21</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>107</v>
@@ -4814,25 +4811,25 @@
         <v>25</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4843,7 +4840,7 @@
         <v>21</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>108</v>
@@ -4858,25 +4855,25 @@
         <v>0</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4887,7 +4884,7 @@
         <v>14</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>109</v>
@@ -4902,25 +4899,25 @@
         <v>30</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>148</v>
+        <v>665</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4931,7 +4928,7 @@
         <v>36</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>110</v>
@@ -4946,25 +4943,25 @@
         <v>20</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>603</v>
+        <v>595</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -4975,7 +4972,7 @@
         <v>21</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>97</v>
@@ -4990,25 +4987,25 @@
         <v>30</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -5019,7 +5016,7 @@
         <v>71</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>111</v>
@@ -5034,25 +5031,25 @@
         <v>25</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
       <c r="N55" s="3" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -5063,7 +5060,7 @@
         <v>73</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>112</v>
@@ -5078,25 +5075,25 @@
         <v>25</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -5107,7 +5104,7 @@
         <v>75</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>113</v>
@@ -5122,25 +5119,25 @@
         <v>0</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -5151,7 +5148,7 @@
         <v>77</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>114</v>
@@ -5166,25 +5163,25 @@
         <v>0</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>631</v>
+        <v>623</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>633</v>
+        <v>625</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -5195,7 +5192,7 @@
         <v>19</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>115</v>
@@ -5210,25 +5207,25 @@
         <v>20</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -5239,7 +5236,7 @@
         <v>8</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>116</v>
@@ -5254,25 +5251,25 @@
         <v>0</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -5283,7 +5280,7 @@
         <v>27</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>117</v>
@@ -5298,25 +5295,25 @@
         <v>0</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="N61" s="2" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -5327,7 +5324,7 @@
         <v>38</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>118</v>
@@ -5342,25 +5339,25 @@
         <v>30</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>157</v>
+        <v>662</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -5371,7 +5368,7 @@
         <v>21</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>120</v>
@@ -5386,25 +5383,25 @@
         <v>30</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -5415,7 +5412,7 @@
         <v>7</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>119</v>
@@ -5430,25 +5427,25 @@
         <v>30</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
     </row>
   </sheetData>
@@ -5456,6 +5453,9 @@
     <sortCondition ref="A2:A64"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{2FCFD574-F158-3345-8AF6-1AC414552316}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>